<commit_message>
update report for jdbc
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/test-luopan-rt.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/test-luopan-rt.xlsx
@@ -902,12 +902,15 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -937,9 +940,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1152,80 +1152,80 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>_input!$A$5:$A$28</c:f>
+              <c:f>_input!$E$5:$E$28</c:f>
               <c:strCache>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0:00</c:v>
+                  <c:v>1:00</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1:00</c:v>
+                  <c:v>2:00</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2:00</c:v>
+                  <c:v>3:00</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3:00</c:v>
+                  <c:v>4:00</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4:00</c:v>
+                  <c:v>5:00</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5:00</c:v>
+                  <c:v>6:00</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6:00</c:v>
+                  <c:v>7:00</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7:00</c:v>
+                  <c:v>8:00</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8:00</c:v>
+                  <c:v>9:00</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9:00</c:v>
+                  <c:v>10:00</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10:00</c:v>
+                  <c:v>11:00</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11:00</c:v>
+                  <c:v>12:00</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12:00</c:v>
+                  <c:v>13:00</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13:00</c:v>
+                  <c:v>14:00</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14:00</c:v>
+                  <c:v>15:00</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15:00</c:v>
+                  <c:v>16:00</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16:00</c:v>
+                  <c:v>17:00</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17:00</c:v>
+                  <c:v>18:00</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18:00</c:v>
+                  <c:v>19:00</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19:00</c:v>
+                  <c:v>20:00</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20:00</c:v>
+                  <c:v>21:00</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21:00</c:v>
+                  <c:v>22:00</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22:00</c:v>
+                  <c:v>23:00</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23:00</c:v>
+                  <c:v>24:00</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1328,80 +1328,80 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>_input!$A$5:$A$28</c:f>
+              <c:f>_input!$E$5:$E$28</c:f>
               <c:strCache>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0:00</c:v>
+                  <c:v>1:00</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1:00</c:v>
+                  <c:v>2:00</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2:00</c:v>
+                  <c:v>3:00</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3:00</c:v>
+                  <c:v>4:00</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4:00</c:v>
+                  <c:v>5:00</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5:00</c:v>
+                  <c:v>6:00</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6:00</c:v>
+                  <c:v>7:00</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7:00</c:v>
+                  <c:v>8:00</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8:00</c:v>
+                  <c:v>9:00</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9:00</c:v>
+                  <c:v>10:00</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10:00</c:v>
+                  <c:v>11:00</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11:00</c:v>
+                  <c:v>12:00</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12:00</c:v>
+                  <c:v>13:00</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13:00</c:v>
+                  <c:v>14:00</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14:00</c:v>
+                  <c:v>15:00</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15:00</c:v>
+                  <c:v>16:00</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16:00</c:v>
+                  <c:v>17:00</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17:00</c:v>
+                  <c:v>18:00</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18:00</c:v>
+                  <c:v>19:00</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19:00</c:v>
+                  <c:v>20:00</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20:00</c:v>
+                  <c:v>21:00</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21:00</c:v>
+                  <c:v>22:00</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22:00</c:v>
+                  <c:v>23:00</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23:00</c:v>
+                  <c:v>24:00</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1504,80 +1504,80 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>_input!$A$5:$A$28</c:f>
+              <c:f>_input!$E$5:$E$28</c:f>
               <c:strCache>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0:00</c:v>
+                  <c:v>1:00</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1:00</c:v>
+                  <c:v>2:00</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2:00</c:v>
+                  <c:v>3:00</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3:00</c:v>
+                  <c:v>4:00</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4:00</c:v>
+                  <c:v>5:00</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5:00</c:v>
+                  <c:v>6:00</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6:00</c:v>
+                  <c:v>7:00</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7:00</c:v>
+                  <c:v>8:00</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8:00</c:v>
+                  <c:v>9:00</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9:00</c:v>
+                  <c:v>10:00</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10:00</c:v>
+                  <c:v>11:00</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11:00</c:v>
+                  <c:v>12:00</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12:00</c:v>
+                  <c:v>13:00</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13:00</c:v>
+                  <c:v>14:00</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14:00</c:v>
+                  <c:v>15:00</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15:00</c:v>
+                  <c:v>16:00</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16:00</c:v>
+                  <c:v>17:00</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17:00</c:v>
+                  <c:v>18:00</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18:00</c:v>
+                  <c:v>19:00</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19:00</c:v>
+                  <c:v>20:00</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20:00</c:v>
+                  <c:v>21:00</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21:00</c:v>
+                  <c:v>22:00</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22:00</c:v>
+                  <c:v>23:00</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23:00</c:v>
+                  <c:v>24:00</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1665,11 +1665,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="78081024"/>
-        <c:axId val="78099200"/>
+        <c:axId val="78801536"/>
+        <c:axId val="78819712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78081024"/>
+        <c:axId val="78801536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1678,14 +1678,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78099200"/>
+        <c:crossAx val="78819712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78099200"/>
+        <c:axId val="78819712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1694,7 +1694,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78081024"/>
+        <c:crossAx val="78801536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1712,7 +1712,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000844" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000844" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000866" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000866" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2082,17 +2082,17 @@
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="2:17">
-      <c r="B2" s="42" t="str">
+      <c r="B2" s="43" t="str">
         <f>_input!$A2&amp;"+"&amp;_input!$A3&amp;"+趋势图"</f>
         <v>商业产品线+分析指标+趋势图</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="2:17">
@@ -2165,17 +2165,17 @@
       <c r="Q23" s="5"/>
     </row>
     <row r="24" spans="1:27">
-      <c r="B24" s="42" t="str">
+      <c r="B24" s="43" t="str">
         <f>_input!$B3&amp;"分小时数据表"</f>
         <v>点击消费分小时数据表</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
       <c r="Q24" s="5"/>
       <c r="V24" t="s">
         <v>24</v>
@@ -2211,22 +2211,22 @@
       <c r="AA26" s="20"/>
     </row>
     <row r="27" spans="1:27" ht="35.25" customHeight="1">
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="37" t="s">
+      <c r="C27" s="45"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="40"/>
       <c r="N27" s="27" t="s">
         <v>54</v>
       </c>
@@ -2236,15 +2236,15 @@
       <c r="R27" s="28"/>
       <c r="S27" s="28"/>
       <c r="T27" s="29"/>
-      <c r="U27" s="40" t="s">
+      <c r="U27" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="V27" s="38"/>
-      <c r="W27" s="38"/>
-      <c r="X27" s="38"/>
-      <c r="Y27" s="38"/>
-      <c r="Z27" s="38"/>
-      <c r="AA27" s="41"/>
+      <c r="V27" s="39"/>
+      <c r="W27" s="39"/>
+      <c r="X27" s="39"/>
+      <c r="Y27" s="39"/>
+      <c r="Z27" s="39"/>
+      <c r="AA27" s="42"/>
     </row>
     <row r="28" spans="1:27" ht="16.5" customHeight="1">
       <c r="A28" s="26" t="s">
@@ -2267,7 +2267,7 @@
       <c r="K28" s="34"/>
       <c r="L28" s="34"/>
       <c r="M28" s="23"/>
-      <c r="N28" s="35">
+      <c r="N28" s="37">
         <f>_input!$C5</f>
         <v>3224110</v>
       </c>
@@ -2287,7 +2287,7 @@
         <f>_input!$F5</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U28" s="47">
+      <c r="U28" s="35">
         <f>_input!$D5</f>
         <v>3334440</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="K29" s="34"/>
       <c r="L29" s="34"/>
       <c r="M29" s="23"/>
-      <c r="N29" s="35">
+      <c r="N29" s="37">
         <f>_input!$C6</f>
         <v>4343110</v>
       </c>
@@ -2349,7 +2349,7 @@
         <f>_input!$F6</f>
         <v>-0.23485474694401021</v>
       </c>
-      <c r="U29" s="47">
+      <c r="U29" s="35">
         <f>_input!$D6</f>
         <v>3323440</v>
       </c>
@@ -2391,7 +2391,7 @@
       <c r="K30" s="34"/>
       <c r="L30" s="34"/>
       <c r="M30" s="23"/>
-      <c r="N30" s="35">
+      <c r="N30" s="37">
         <f>_input!$C7</f>
         <v>3224110</v>
       </c>
@@ -2411,7 +2411,7 @@
         <f>_input!$F7</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U30" s="47">
+      <c r="U30" s="35">
         <f>_input!$D7</f>
         <v>3324440</v>
       </c>
@@ -2453,7 +2453,7 @@
       <c r="K31" s="34"/>
       <c r="L31" s="34"/>
       <c r="M31" s="23"/>
-      <c r="N31" s="35">
+      <c r="N31" s="37">
         <f>_input!$C8</f>
         <v>3224110</v>
       </c>
@@ -2473,7 +2473,7 @@
         <f>_input!$F8</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U31" s="47">
+      <c r="U31" s="35">
         <f>_input!$D8</f>
         <v>3334440</v>
       </c>
@@ -2515,7 +2515,7 @@
       <c r="K32" s="34"/>
       <c r="L32" s="34"/>
       <c r="M32" s="23"/>
-      <c r="N32" s="35">
+      <c r="N32" s="37">
         <f>_input!$C9</f>
         <v>3664110</v>
       </c>
@@ -2535,7 +2535,7 @@
         <f>_input!$F9</f>
         <v>-8.7333622625958229E-2</v>
       </c>
-      <c r="U32" s="47">
+      <c r="U32" s="35">
         <f>_input!$D9</f>
         <v>3244440</v>
       </c>
@@ -2577,7 +2577,7 @@
       <c r="K33" s="34"/>
       <c r="L33" s="34"/>
       <c r="M33" s="23"/>
-      <c r="N33" s="35">
+      <c r="N33" s="37">
         <f>_input!$C10</f>
         <v>3224110</v>
       </c>
@@ -2597,7 +2597,7 @@
         <f>_input!$F10</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U33" s="47">
+      <c r="U33" s="35">
         <f>_input!$D10</f>
         <v>3334440</v>
       </c>
@@ -2639,7 +2639,7 @@
       <c r="K34" s="34"/>
       <c r="L34" s="34"/>
       <c r="M34" s="23"/>
-      <c r="N34" s="35">
+      <c r="N34" s="37">
         <f>_input!$C11</f>
         <v>4324110</v>
       </c>
@@ -2659,7 +2659,7 @@
         <f>_input!$F11</f>
         <v>4.6252292379240778E-3</v>
       </c>
-      <c r="U34" s="47">
+      <c r="U34" s="35">
         <f>_input!$D11</f>
         <v>3334440</v>
       </c>
@@ -2701,7 +2701,7 @@
       <c r="K35" s="34"/>
       <c r="L35" s="34"/>
       <c r="M35" s="23"/>
-      <c r="N35" s="35">
+      <c r="N35" s="37">
         <f>_input!$C12</f>
         <v>3224110</v>
       </c>
@@ -2721,7 +2721,7 @@
         <f>_input!$F12</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U35" s="47">
+      <c r="U35" s="35">
         <f>_input!$D12</f>
         <v>3554440</v>
       </c>
@@ -2763,7 +2763,7 @@
       <c r="K36" s="34"/>
       <c r="L36" s="34"/>
       <c r="M36" s="23"/>
-      <c r="N36" s="35">
+      <c r="N36" s="37">
         <f>_input!$C13</f>
         <v>3224110</v>
       </c>
@@ -2783,7 +2783,7 @@
         <f>_input!$F13</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U36" s="47">
+      <c r="U36" s="35">
         <f>_input!$D13</f>
         <v>3674440</v>
       </c>
@@ -2825,7 +2825,7 @@
       <c r="K37" s="34"/>
       <c r="L37" s="34"/>
       <c r="M37" s="23"/>
-      <c r="N37" s="35">
+      <c r="N37" s="37">
         <f>_input!$C14</f>
         <v>3224110</v>
       </c>
@@ -2845,7 +2845,7 @@
         <f>_input!$F14</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U37" s="47">
+      <c r="U37" s="35">
         <f>_input!$D14</f>
         <v>3334440</v>
       </c>
@@ -2887,7 +2887,7 @@
       <c r="K38" s="34"/>
       <c r="L38" s="34"/>
       <c r="M38" s="23"/>
-      <c r="N38" s="35">
+      <c r="N38" s="37">
         <f>_input!$C15</f>
         <v>3524110</v>
       </c>
@@ -2907,7 +2907,7 @@
         <f>_input!$F15</f>
         <v>-5.1076725754871433E-2</v>
       </c>
-      <c r="U38" s="47">
+      <c r="U38" s="35">
         <f>_input!$D15</f>
         <v>3544440</v>
       </c>
@@ -2949,7 +2949,7 @@
       <c r="K39" s="34"/>
       <c r="L39" s="34"/>
       <c r="M39" s="23"/>
-      <c r="N39" s="35">
+      <c r="N39" s="37">
         <f>_input!$C16</f>
         <v>3224110</v>
       </c>
@@ -2969,7 +2969,7 @@
         <f>_input!$F16</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U39" s="47">
+      <c r="U39" s="35">
         <f>_input!$D16</f>
         <v>3334440</v>
       </c>
@@ -3011,7 +3011,7 @@
       <c r="K40" s="34"/>
       <c r="L40" s="34"/>
       <c r="M40" s="23"/>
-      <c r="N40" s="35">
+      <c r="N40" s="37">
         <f>_input!$C17</f>
         <v>3224110</v>
       </c>
@@ -3031,7 +3031,7 @@
         <f>_input!$F17</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U40" s="47">
+      <c r="U40" s="35">
         <f>_input!$D17</f>
         <v>3334440</v>
       </c>
@@ -3073,7 +3073,7 @@
       <c r="K41" s="34"/>
       <c r="L41" s="34"/>
       <c r="M41" s="23"/>
-      <c r="N41" s="35">
+      <c r="N41" s="37">
         <f>_input!$C18</f>
         <v>3224110</v>
       </c>
@@ -3093,7 +3093,7 @@
         <f>_input!$F18</f>
         <v>8.0642409843336704E-2</v>
       </c>
-      <c r="U41" s="47">
+      <c r="U41" s="35">
         <f>_input!$D18</f>
         <v>3344440</v>
       </c>
@@ -3135,7 +3135,7 @@
       <c r="K42" s="34"/>
       <c r="L42" s="34"/>
       <c r="M42" s="23"/>
-      <c r="N42" s="35">
+      <c r="N42" s="37">
         <f>_input!$C19</f>
         <v>3224110</v>
       </c>
@@ -3155,7 +3155,7 @@
         <f>_input!$F19</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U42" s="47">
+      <c r="U42" s="35">
         <f>_input!$D19</f>
         <v>3334440</v>
       </c>
@@ -3197,7 +3197,7 @@
       <c r="K43" s="34"/>
       <c r="L43" s="34"/>
       <c r="M43" s="23"/>
-      <c r="N43" s="35">
+      <c r="N43" s="37">
         <f>_input!$C20</f>
         <v>3224110</v>
       </c>
@@ -3217,7 +3217,7 @@
         <f>_input!$F20</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U43" s="47">
+      <c r="U43" s="35">
         <f>_input!$D20</f>
         <v>3544440</v>
       </c>
@@ -3259,7 +3259,7 @@
       <c r="K44" s="34"/>
       <c r="L44" s="34"/>
       <c r="M44" s="23"/>
-      <c r="N44" s="35">
+      <c r="N44" s="37">
         <f>_input!$C21</f>
         <v>3434110</v>
       </c>
@@ -3279,7 +3279,7 @@
         <f>_input!$F21</f>
         <v>-2.6207663703259332E-2</v>
       </c>
-      <c r="U44" s="47">
+      <c r="U44" s="35">
         <f>_input!$D21</f>
         <v>3334440</v>
       </c>
@@ -3321,7 +3321,7 @@
       <c r="K45" s="34"/>
       <c r="L45" s="34"/>
       <c r="M45" s="23"/>
-      <c r="N45" s="35">
+      <c r="N45" s="37">
         <f>_input!$C22</f>
         <v>3224110</v>
       </c>
@@ -3341,7 +3341,7 @@
         <f>_input!$F22</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U45" s="47">
+      <c r="U45" s="35">
         <f>_input!$D22</f>
         <v>3334440</v>
       </c>
@@ -3383,7 +3383,7 @@
       <c r="K46" s="34"/>
       <c r="L46" s="34"/>
       <c r="M46" s="23"/>
-      <c r="N46" s="35">
+      <c r="N46" s="37">
         <f>_input!$C23</f>
         <v>3224110</v>
       </c>
@@ -3403,7 +3403,7 @@
         <f>_input!$F23</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U46" s="47">
+      <c r="U46" s="35">
         <f>_input!$D23</f>
         <v>3334440</v>
       </c>
@@ -3445,7 +3445,7 @@
       <c r="K47" s="34"/>
       <c r="L47" s="34"/>
       <c r="M47" s="23"/>
-      <c r="N47" s="35">
+      <c r="N47" s="37">
         <f>_input!$C24</f>
         <v>3224110</v>
       </c>
@@ -3465,7 +3465,7 @@
         <f>_input!$F24</f>
         <v>-0.33497616396462904</v>
       </c>
-      <c r="U47" s="47">
+      <c r="U47" s="35">
         <f>_input!$D24</f>
         <v>3334440</v>
       </c>
@@ -3507,7 +3507,7 @@
       <c r="K48" s="34"/>
       <c r="L48" s="34"/>
       <c r="M48" s="23"/>
-      <c r="N48" s="35">
+      <c r="N48" s="37">
         <f>_input!$C25</f>
         <v>3224110</v>
       </c>
@@ -3527,7 +3527,7 @@
         <f>_input!$F25</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U48" s="47">
+      <c r="U48" s="35">
         <f>_input!$D25</f>
         <v>3334440</v>
       </c>
@@ -3569,7 +3569,7 @@
       <c r="K49" s="34"/>
       <c r="L49" s="34"/>
       <c r="M49" s="23"/>
-      <c r="N49" s="35">
+      <c r="N49" s="37">
         <f>_input!$C26</f>
         <v>3224110</v>
       </c>
@@ -3589,7 +3589,7 @@
         <f>_input!$F26</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U49" s="47">
+      <c r="U49" s="35">
         <f>_input!$D26</f>
         <v>3334440</v>
       </c>
@@ -3631,7 +3631,7 @@
       <c r="K50" s="34"/>
       <c r="L50" s="34"/>
       <c r="M50" s="23"/>
-      <c r="N50" s="35">
+      <c r="N50" s="37">
         <f>_input!$C27</f>
         <v>3994110</v>
       </c>
@@ -3651,7 +3651,7 @@
         <f>_input!$F27</f>
         <v>-0.16273963411122883</v>
       </c>
-      <c r="U50" s="47">
+      <c r="U50" s="35">
         <f>_input!$D27</f>
         <v>3334440</v>
       </c>
@@ -3693,7 +3693,7 @@
       <c r="K51" s="34"/>
       <c r="L51" s="34"/>
       <c r="M51" s="23"/>
-      <c r="N51" s="35">
+      <c r="N51" s="37">
         <f>_input!$C28</f>
         <v>3224110</v>
       </c>
@@ -3713,7 +3713,7 @@
         <f>_input!$F28</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="U51" s="47">
+      <c r="U51" s="35">
         <f>_input!$D28</f>
         <v>3214440</v>
       </c>
@@ -4027,7 +4027,7 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="13.75" customWidth="1"/>
-    <col min="5" max="5" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.25" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="9.25" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.25" bestFit="1" customWidth="1"/>
@@ -4081,6 +4081,10 @@
       <c r="D5" s="3">
         <v>3334440</v>
       </c>
+      <c r="E5" s="18" t="str">
+        <f>(VALUE(LEFT($A5,LEN($A5)-3)) + 1) &amp;":00"</f>
+        <v>1:00</v>
+      </c>
       <c r="F5" s="19">
         <f>$B5/$C5-1</f>
         <v>3.7219573773847658E-2</v>
@@ -4103,12 +4107,16 @@
       <c r="D6" s="3">
         <v>3323440</v>
       </c>
+      <c r="E6" s="18" t="str">
+        <f t="shared" ref="E6:E28" si="0">(VALUE(LEFT($A6,LEN($A6)-3)) + 1) &amp;":00"</f>
+        <v>2:00</v>
+      </c>
       <c r="F6" s="19">
-        <f t="shared" ref="F6:F28" si="0">$B6/$C6-1</f>
+        <f t="shared" ref="F6:F28" si="1">$B6/$C6-1</f>
         <v>-0.23485474694401021</v>
       </c>
       <c r="G6" s="19">
-        <f t="shared" ref="G6:G28" si="1">$B6/$D6-1</f>
+        <f t="shared" ref="G6:G28" si="2">$B6/$D6-1</f>
         <v>-9.9294706689456724E-5</v>
       </c>
     </row>
@@ -4125,12 +4133,16 @@
       <c r="D7" s="3">
         <v>3324440</v>
       </c>
+      <c r="E7" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>3:00</v>
+      </c>
       <c r="F7" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G7" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.9167859850079996E-3</v>
       </c>
     </row>
@@ -4147,12 +4159,16 @@
       <c r="D8" s="3">
         <v>3334440</v>
       </c>
+      <c r="E8" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>4:00</v>
+      </c>
       <c r="F8" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G8" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
@@ -4169,12 +4185,16 @@
       <c r="D9" s="3">
         <v>3244440</v>
       </c>
+      <c r="E9" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>5:00</v>
+      </c>
       <c r="F9" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-8.7333622625958229E-2</v>
       </c>
       <c r="G9" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.0720247561982994E-2</v>
       </c>
     </row>
@@ -4191,12 +4211,16 @@
       <c r="D10" s="3">
         <v>3334440</v>
       </c>
+      <c r="E10" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>6:00</v>
+      </c>
       <c r="F10" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G10" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
@@ -4213,12 +4237,16 @@
       <c r="D11" s="3">
         <v>3334440</v>
       </c>
+      <c r="E11" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>7:00</v>
+      </c>
       <c r="F11" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.6252292379240778E-3</v>
       </c>
       <c r="G11" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.30280047024387913</v>
       </c>
     </row>
@@ -4235,12 +4263,16 @@
       <c r="D12" s="3">
         <v>3554440</v>
       </c>
+      <c r="E12" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>8:00</v>
+      </c>
       <c r="F12" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G12" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.9173878304317973E-2</v>
       </c>
     </row>
@@ -4257,12 +4289,16 @@
       <c r="D13" s="3">
         <v>3674440</v>
       </c>
+      <c r="E13" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>9:00</v>
+      </c>
       <c r="F13" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G13" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-8.9899413243922921E-2</v>
       </c>
     </row>
@@ -4279,12 +4315,16 @@
       <c r="D14" s="3">
         <v>3334440</v>
       </c>
+      <c r="E14" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>10:00</v>
+      </c>
       <c r="F14" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G14" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
@@ -4301,12 +4341,16 @@
       <c r="D15" s="3">
         <v>3544440</v>
       </c>
+      <c r="E15" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>11:00</v>
+      </c>
       <c r="F15" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-5.1076725754871433E-2</v>
       </c>
       <c r="G15" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.65195066075318E-2</v>
       </c>
     </row>
@@ -4323,12 +4367,16 @@
       <c r="D16" s="3">
         <v>3334440</v>
       </c>
+      <c r="E16" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>12:00</v>
+      </c>
       <c r="F16" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G16" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
@@ -4345,12 +4393,16 @@
       <c r="D17" s="3">
         <v>3334440</v>
       </c>
+      <c r="E17" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>13:00</v>
+      </c>
       <c r="F17" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G17" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
@@ -4367,12 +4419,16 @@
       <c r="D18" s="3">
         <v>3344440</v>
       </c>
+      <c r="E18" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>14:00</v>
+      </c>
       <c r="F18" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.0642409843336704E-2</v>
       </c>
       <c r="G18" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.1761849517407912E-2</v>
       </c>
     </row>
@@ -4389,12 +4445,16 @@
       <c r="D19" s="3">
         <v>3334440</v>
       </c>
+      <c r="E19" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>15:00</v>
+      </c>
       <c r="F19" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G19" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
@@ -4411,12 +4471,16 @@
       <c r="D20" s="3">
         <v>3544440</v>
       </c>
+      <c r="E20" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>16:00</v>
+      </c>
       <c r="F20" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G20" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.65195066075318E-2</v>
       </c>
     </row>
@@ -4433,12 +4497,16 @@
       <c r="D21" s="3">
         <v>3334440</v>
       </c>
+      <c r="E21" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>17:00</v>
+      </c>
       <c r="F21" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.6207663703259332E-2</v>
       </c>
       <c r="G21" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
@@ -4455,12 +4523,16 @@
       <c r="D22" s="3">
         <v>3334440</v>
       </c>
+      <c r="E22" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>18:00</v>
+      </c>
       <c r="F22" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G22" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
@@ -4477,12 +4549,16 @@
       <c r="D23" s="3">
         <v>3334440</v>
       </c>
+      <c r="E23" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>19:00</v>
+      </c>
       <c r="F23" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G23" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
@@ -4499,12 +4575,16 @@
       <c r="D24" s="3">
         <v>3334440</v>
       </c>
+      <c r="E24" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>20:00</v>
+      </c>
       <c r="F24" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.33497616396462904</v>
       </c>
       <c r="G24" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.35698048247981673</v>
       </c>
     </row>
@@ -4521,12 +4601,16 @@
       <c r="D25" s="3">
         <v>3334440</v>
       </c>
+      <c r="E25" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>21:00</v>
+      </c>
       <c r="F25" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G25" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
@@ -4543,12 +4627,16 @@
       <c r="D26" s="3">
         <v>3334440</v>
       </c>
+      <c r="E26" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>22:00</v>
+      </c>
       <c r="F26" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G26" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
@@ -4565,12 +4653,16 @@
       <c r="D27" s="3">
         <v>3334440</v>
       </c>
+      <c r="E27" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>23:00</v>
+      </c>
       <c r="F27" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.16273963411122883</v>
       </c>
       <c r="G27" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
@@ -4587,12 +4679,16 @@
       <c r="D28" s="3">
         <v>3214440</v>
       </c>
+      <c r="E28" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>24:00</v>
+      </c>
       <c r="F28" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7219573773847658E-2</v>
       </c>
       <c r="G28" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.0339841465387494E-2</v>
       </c>
     </row>

</xml_diff>